<commit_message>
Zeiterfasung und GDD Update
</commit_message>
<xml_diff>
--- a/_WIP/Tobias/Tobias-Zeiterfassung.xlsx
+++ b/_WIP/Tobias/Tobias-Zeiterfassung.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="148">
   <si>
     <t>Zeiterfassung</t>
   </si>
@@ -460,6 +460,10 @@
   </si>
   <si>
     <t>Dokumentation Mechaniken, Level Design</t>
+  </si>
+  <si>
+    <t>Whitebox für Level 1;
+Level Design mit Artjom besprochen</t>
   </si>
 </sst>
 </file>
@@ -1049,7 +1053,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1059,8 +1063,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H184"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="G47" sqref="G47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1874,19 +1878,27 @@
         <v>10</v>
       </c>
     </row>
-    <row r="46" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B46" s="13"/>
-      <c r="C46" s="13"/>
-      <c r="D46" s="24"/>
+      <c r="B46" s="13">
+        <v>0.40625</v>
+      </c>
+      <c r="C46" s="13">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="D46" s="24">
+        <v>1.5</v>
+      </c>
       <c r="E46" s="9">
         <f>(B46-C46)*-24-D46</f>
-        <v>0</v>
+        <v>5.7500000000000009</v>
       </c>
       <c r="F46" s="12"/>
-      <c r="G46" s="12"/>
+      <c r="G46" s="12" t="s">
+        <v>147</v>
+      </c>
       <c r="H46" s="12"/>
     </row>
     <row r="47" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1988,7 +2000,7 @@
       </c>
       <c r="E53" s="22">
         <f>SUM(E46:E52)</f>
-        <v>0</v>
+        <v>5.7500000000000009</v>
       </c>
       <c r="F53" s="2"/>
       <c r="G53" s="2"/>
@@ -2003,7 +2015,7 @@
       </c>
       <c r="E54" s="23">
         <f>SUM(E13+E23+E33+E43+E53)</f>
-        <v>69.083333333333343</v>
+        <v>74.833333333333343</v>
       </c>
       <c r="F54" s="3"/>
       <c r="G54" s="3"/>
@@ -2164,7 +2176,7 @@
       </c>
       <c r="E64" s="23">
         <f>SUM(E13+E23+E33+E43+E53+E63)</f>
-        <v>69.083333333333343</v>
+        <v>74.833333333333343</v>
       </c>
       <c r="F64" s="3"/>
       <c r="G64" s="3"/>
@@ -2325,7 +2337,7 @@
       </c>
       <c r="E74" s="23">
         <f>SUM(E13+E23+E33+E43+E53+E63+E73)</f>
-        <v>69.083333333333343</v>
+        <v>74.833333333333343</v>
       </c>
       <c r="F74" s="3"/>
       <c r="G74" s="3"/>
@@ -2486,7 +2498,7 @@
       </c>
       <c r="E84" s="23">
         <f>SUM(E13+E23+E33+E43+E53+E63+E73+E83)</f>
-        <v>69.083333333333343</v>
+        <v>74.833333333333343</v>
       </c>
       <c r="F84" s="3"/>
       <c r="G84" s="3"/>
@@ -2647,7 +2659,7 @@
       </c>
       <c r="E94" s="23">
         <f>SUM(E13+E23+E33+E43+E53+E63+E73+E83+E93)</f>
-        <v>69.083333333333343</v>
+        <v>74.833333333333343</v>
       </c>
       <c r="F94" s="3"/>
       <c r="G94" s="3"/>
@@ -2808,7 +2820,7 @@
       </c>
       <c r="E104" s="23">
         <f>SUM(E13+E23+E33+E43+E53+E63+E73+E83+E93+E103)</f>
-        <v>69.083333333333343</v>
+        <v>74.833333333333343</v>
       </c>
       <c r="F104" s="3"/>
       <c r="G104" s="3"/>
@@ -2969,7 +2981,7 @@
       </c>
       <c r="E114" s="23">
         <f>SUM(E13+E23+E33+E43+E53+E63+E73+E83+E93+E103+E113)</f>
-        <v>69.083333333333343</v>
+        <v>74.833333333333343</v>
       </c>
       <c r="F114" s="3"/>
       <c r="G114" s="3"/>
@@ -3130,7 +3142,7 @@
       </c>
       <c r="E124" s="23">
         <f>SUM(E13+E23+E33+E43+E53+E63+E73+E83+E93+E103+E113+E123)</f>
-        <v>69.083333333333343</v>
+        <v>74.833333333333343</v>
       </c>
       <c r="F124" s="3"/>
       <c r="G124" s="3"/>
@@ -3291,7 +3303,7 @@
       </c>
       <c r="E134" s="23">
         <f>SUM(E13+E23+E33+E43+E53+E63+E73+E83+E93+E103+E113+E123+E133)</f>
-        <v>69.083333333333343</v>
+        <v>74.833333333333343</v>
       </c>
       <c r="F134" s="3"/>
       <c r="G134" s="3"/>
@@ -3452,7 +3464,7 @@
       </c>
       <c r="E144" s="23">
         <f>SUM(E13+E23+E33+E43+E53+E63+E73+E83+E93+E103+E113+E123+E133+E143)</f>
-        <v>69.083333333333343</v>
+        <v>74.833333333333343</v>
       </c>
       <c r="F144" s="3"/>
       <c r="G144" s="3"/>
@@ -3613,7 +3625,7 @@
       </c>
       <c r="E154" s="23">
         <f>SUM(E13+E23+E33+E43+E53+E63+E73+E83+E93+E103+E113+E123+E133+E143+E153)</f>
-        <v>69.083333333333343</v>
+        <v>74.833333333333343</v>
       </c>
       <c r="F154" s="3"/>
       <c r="G154" s="3"/>
@@ -3773,7 +3785,7 @@
       </c>
       <c r="E164" s="23">
         <f>SUM(E13+E23+E33+E43+E53+E63+E73+E83+E93+E103+E113+E123+E133+E143+E153+E163)</f>
-        <v>69.083333333333343</v>
+        <v>74.833333333333343</v>
       </c>
       <c r="F164" s="3"/>
       <c r="G164" s="3"/>
@@ -3934,7 +3946,7 @@
       </c>
       <c r="E174" s="23">
         <f>SUM(E13+E23+E33+E43+E53+E63+E73+E83+E93+E103+E113+E123+E133+E143+E153+E163+E173)</f>
-        <v>69.083333333333343</v>
+        <v>74.833333333333343</v>
       </c>
       <c r="F174" s="3"/>
       <c r="G174" s="3"/>
@@ -4095,7 +4107,7 @@
       </c>
       <c r="E184" s="28">
         <f>SUM(E13+E23+E33+E43+E53+E63+E73+E83+E93+E103+E113+E123+E133+E143+E153+E163+E173+E183)</f>
-        <v>69.083333333333343</v>
+        <v>74.833333333333343</v>
       </c>
       <c r="F184" s="2"/>
       <c r="G184" s="2"/>

</xml_diff>